<commit_message>
SQL-2 Zad 10 update
</commit_message>
<xml_diff>
--- a/praca_domowa_2/wa_9.xlsx
+++ b/praca_domowa_2/wa_9.xlsx
@@ -129,7 +129,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -216,11 +215,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="171946368"/>
-        <c:axId val="174787968"/>
+        <c:axId val="107241472"/>
+        <c:axId val="107243008"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="171946368"/>
+        <c:axId val="107241472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -229,7 +228,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="174787968"/>
+        <c:crossAx val="107243008"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -237,7 +236,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="174787968"/>
+        <c:axId val="107243008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -260,14 +259,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="171946368"/>
+        <c:crossAx val="107241472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -688,724 +686,1120 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D132"/>
+  <dimension ref="A1:G132"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A1:A18"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>10</v>
+        <v>384</v>
       </c>
       <c r="D1">
         <v>384</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>6649</v>
+        <v>11760</v>
       </c>
       <c r="D2">
         <v>11760</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G2">
+        <v>6.0000000000000002E-5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2825</v>
+        <v>120</v>
       </c>
       <c r="D3">
         <v>120</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G3">
+        <v>3.6990000000000002E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>98</v>
+        <v>192</v>
       </c>
       <c r="D4">
         <v>192</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G4">
+        <v>1.5689999999999999E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>145134</v>
+        <v>48</v>
       </c>
       <c r="D5">
         <v>48</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G5">
+        <v>5.5000000000000003E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>1668</v>
+        <v>120</v>
       </c>
       <c r="D6">
         <v>120</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G6">
+        <v>0.80749000000000004</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>2105</v>
+        <v>144</v>
       </c>
       <c r="D7">
         <v>144</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G7">
+        <v>9.2899999999999996E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>982</v>
+        <v>912</v>
       </c>
       <c r="D8">
         <v>912</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G8">
+        <v>1.171E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>1990</v>
+        <v>288</v>
       </c>
       <c r="D9">
         <v>288</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G9">
+        <v>5.4799999999999996E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>2572</v>
+        <v>48</v>
       </c>
       <c r="D10">
         <v>48</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G10">
+        <v>1.1089999999999999E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>265</v>
+        <v>240</v>
       </c>
       <c r="D11">
         <v>240</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G11">
+        <v>1.4330000000000001E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>1</v>
+        <v>384</v>
       </c>
       <c r="D12">
         <v>384</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G12">
+        <v>1.48E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>7973</v>
+        <v>7840</v>
       </c>
       <c r="D13">
         <v>7840</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G13">
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>3333</v>
+        <v>80</v>
       </c>
       <c r="D14">
         <v>80</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G14">
+        <v>4.4299999999999999E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>72</v>
+        <v>128</v>
       </c>
       <c r="D15">
         <v>128</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G15">
+        <v>1.8550000000000001E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>544</v>
+        <v>32</v>
       </c>
       <c r="D16">
         <v>32</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G16">
+        <v>4.0000000000000002E-4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>3479</v>
+        <v>80</v>
       </c>
       <c r="D17">
         <v>80</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G17">
+        <v>3.0300000000000001E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>35</v>
+        <v>96</v>
       </c>
       <c r="D18">
         <v>96</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G18">
+        <v>1.9369999999999998E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>608</v>
+      </c>
       <c r="D19">
         <v>608</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G19">
+        <v>2.0000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>192</v>
+      </c>
       <c r="D20">
         <v>192</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>32</v>
+      </c>
       <c r="D21">
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>160</v>
+      </c>
       <c r="D22">
         <v>160</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>11760</v>
+      </c>
       <c r="D23">
         <v>11760</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>7840</v>
+      </c>
       <c r="D24">
         <v>7840</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>2450</v>
+      </c>
       <c r="D25">
         <v>2450</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>3920</v>
+      </c>
       <c r="D26">
         <v>3920</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>980</v>
+      </c>
       <c r="D27">
         <v>980</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>2450</v>
+      </c>
       <c r="D28">
         <v>2450</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>2940</v>
+      </c>
       <c r="D29">
         <v>2940</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>18620</v>
+      </c>
       <c r="D30">
         <v>18620</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>5880</v>
+      </c>
       <c r="D31">
         <v>5880</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>980</v>
+      </c>
       <c r="D32">
         <v>980</v>
       </c>
     </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>4900</v>
+      </c>
       <c r="D33">
         <v>4900</v>
       </c>
     </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>120</v>
+      </c>
       <c r="D34">
         <v>120</v>
       </c>
     </row>
-    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>80</v>
+      </c>
       <c r="D35">
         <v>80</v>
       </c>
     </row>
-    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>2450</v>
+      </c>
       <c r="D36">
         <v>2450</v>
       </c>
     </row>
-    <row r="37" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>40</v>
+      </c>
       <c r="D37">
         <v>40</v>
       </c>
     </row>
-    <row r="38" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>10</v>
+      </c>
       <c r="D38">
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>25</v>
+      </c>
       <c r="D39">
         <v>25</v>
       </c>
     </row>
-    <row r="40" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>30</v>
+      </c>
       <c r="D40">
         <v>30</v>
       </c>
     </row>
-    <row r="41" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>190</v>
+      </c>
       <c r="D41">
         <v>190</v>
       </c>
     </row>
-    <row r="42" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>60</v>
+      </c>
       <c r="D42">
         <v>60</v>
       </c>
     </row>
-    <row r="43" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>10</v>
+      </c>
       <c r="D43">
         <v>10</v>
       </c>
     </row>
-    <row r="44" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>50</v>
+      </c>
       <c r="D44">
         <v>50</v>
       </c>
     </row>
-    <row r="45" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>192</v>
+      </c>
       <c r="D45">
         <v>192</v>
       </c>
     </row>
-    <row r="46" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>128</v>
+      </c>
       <c r="D46">
         <v>128</v>
       </c>
     </row>
-    <row r="47" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>3920</v>
+      </c>
       <c r="D47">
         <v>3920</v>
       </c>
     </row>
-    <row r="48" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>40</v>
+      </c>
       <c r="D48">
         <v>40</v>
       </c>
     </row>
-    <row r="49" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>16</v>
+      </c>
       <c r="D49">
         <v>16</v>
       </c>
     </row>
-    <row r="50" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>40</v>
+      </c>
       <c r="D50">
         <v>40</v>
       </c>
     </row>
-    <row r="51" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>48</v>
+      </c>
       <c r="D51">
         <v>48</v>
       </c>
     </row>
-    <row r="52" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>304</v>
+      </c>
       <c r="D52">
         <v>304</v>
       </c>
     </row>
-    <row r="53" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>96</v>
+      </c>
       <c r="D53">
         <v>96</v>
       </c>
     </row>
-    <row r="54" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>16</v>
+      </c>
       <c r="D54">
         <v>16</v>
       </c>
     </row>
-    <row r="55" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>80</v>
+      </c>
       <c r="D55">
         <v>80</v>
       </c>
     </row>
-    <row r="56" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>48</v>
+      </c>
       <c r="D56">
         <v>48</v>
       </c>
     </row>
-    <row r="57" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>32</v>
+      </c>
       <c r="D57">
         <v>32</v>
       </c>
     </row>
-    <row r="58" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>980</v>
+      </c>
       <c r="D58">
         <v>980</v>
       </c>
     </row>
-    <row r="59" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>10</v>
+      </c>
       <c r="D59">
         <v>10</v>
       </c>
     </row>
-    <row r="60" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>16</v>
+      </c>
       <c r="D60">
         <v>16</v>
       </c>
     </row>
-    <row r="61" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>10</v>
+      </c>
       <c r="D61">
         <v>10</v>
       </c>
     </row>
-    <row r="62" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>12</v>
+      </c>
       <c r="D62">
         <v>12</v>
       </c>
     </row>
-    <row r="63" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>76</v>
+      </c>
       <c r="D63">
         <v>76</v>
       </c>
     </row>
-    <row r="64" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>24</v>
+      </c>
       <c r="D64">
         <v>24</v>
       </c>
     </row>
-    <row r="65" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>4</v>
+      </c>
       <c r="D65">
         <v>4</v>
       </c>
     </row>
-    <row r="66" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>20</v>
+      </c>
       <c r="D66">
         <v>20</v>
       </c>
     </row>
-    <row r="67" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>120</v>
+      </c>
       <c r="D67">
         <v>120</v>
       </c>
     </row>
-    <row r="68" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>80</v>
+      </c>
       <c r="D68">
         <v>80</v>
       </c>
     </row>
-    <row r="69" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>2450</v>
+      </c>
       <c r="D69">
         <v>2450</v>
       </c>
     </row>
-    <row r="70" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>25</v>
+      </c>
       <c r="D70">
         <v>25</v>
       </c>
     </row>
-    <row r="71" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>40</v>
+      </c>
       <c r="D71">
         <v>40</v>
       </c>
     </row>
-    <row r="72" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>10</v>
+      </c>
       <c r="D72">
         <v>10</v>
       </c>
     </row>
-    <row r="73" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>30</v>
+      </c>
       <c r="D73">
         <v>30</v>
       </c>
     </row>
-    <row r="74" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>190</v>
+      </c>
       <c r="D74">
         <v>190</v>
       </c>
     </row>
-    <row r="75" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>60</v>
+      </c>
       <c r="D75">
         <v>60</v>
       </c>
     </row>
-    <row r="76" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>10</v>
+      </c>
       <c r="D76">
         <v>10</v>
       </c>
     </row>
-    <row r="77" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>50</v>
+      </c>
       <c r="D77">
         <v>50</v>
       </c>
     </row>
-    <row r="78" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>144</v>
+      </c>
       <c r="D78">
         <v>144</v>
       </c>
     </row>
-    <row r="79" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>96</v>
+      </c>
       <c r="D79">
         <v>96</v>
       </c>
     </row>
-    <row r="80" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>2940</v>
+      </c>
       <c r="D80">
         <v>2940</v>
       </c>
     </row>
-    <row r="81" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>30</v>
+      </c>
       <c r="D81">
         <v>30</v>
       </c>
     </row>
-    <row r="82" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>48</v>
+      </c>
       <c r="D82">
         <v>48</v>
       </c>
     </row>
-    <row r="83" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>12</v>
+      </c>
       <c r="D83">
         <v>12</v>
       </c>
     </row>
-    <row r="84" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>30</v>
+      </c>
       <c r="D84">
         <v>30</v>
       </c>
     </row>
-    <row r="85" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>228</v>
+      </c>
       <c r="D85">
         <v>228</v>
       </c>
     </row>
-    <row r="86" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>72</v>
+      </c>
       <c r="D86">
         <v>72</v>
       </c>
     </row>
-    <row r="87" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>12</v>
+      </c>
       <c r="D87">
         <v>12</v>
       </c>
     </row>
-    <row r="88" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>60</v>
+      </c>
       <c r="D88">
         <v>60</v>
       </c>
     </row>
-    <row r="89" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>912</v>
+      </c>
       <c r="D89">
         <v>912</v>
       </c>
     </row>
-    <row r="90" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>608</v>
+      </c>
       <c r="D90">
         <v>608</v>
       </c>
     </row>
-    <row r="91" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>18620</v>
+      </c>
       <c r="D91">
         <v>18620</v>
       </c>
     </row>
-    <row r="92" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>190</v>
+      </c>
       <c r="D92">
         <v>190</v>
       </c>
     </row>
-    <row r="93" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>304</v>
+      </c>
       <c r="D93">
         <v>304</v>
       </c>
     </row>
-    <row r="94" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>76</v>
+      </c>
       <c r="D94">
         <v>76</v>
       </c>
     </row>
-    <row r="95" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>190</v>
+      </c>
       <c r="D95">
         <v>190</v>
       </c>
     </row>
-    <row r="96" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>228</v>
+      </c>
       <c r="D96">
         <v>228</v>
       </c>
     </row>
-    <row r="97" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>456</v>
+      </c>
       <c r="D97">
         <v>456</v>
       </c>
     </row>
-    <row r="98" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>76</v>
+      </c>
       <c r="D98">
         <v>76</v>
       </c>
     </row>
-    <row r="99" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>380</v>
+      </c>
       <c r="D99">
         <v>380</v>
       </c>
     </row>
-    <row r="100" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>288</v>
+      </c>
       <c r="D100">
         <v>288</v>
       </c>
     </row>
-    <row r="101" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>192</v>
+      </c>
       <c r="D101">
         <v>192</v>
       </c>
     </row>
-    <row r="102" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>5880</v>
+      </c>
       <c r="D102">
         <v>5880</v>
       </c>
     </row>
-    <row r="103" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>60</v>
+      </c>
       <c r="D103">
         <v>60</v>
       </c>
     </row>
-    <row r="104" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <v>96</v>
+      </c>
       <c r="D104">
         <v>96</v>
       </c>
     </row>
-    <row r="105" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105">
+        <v>24</v>
+      </c>
       <c r="D105">
         <v>24</v>
       </c>
     </row>
-    <row r="106" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106">
+        <v>60</v>
+      </c>
       <c r="D106">
         <v>60</v>
       </c>
     </row>
-    <row r="107" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <v>72</v>
+      </c>
       <c r="D107">
         <v>72</v>
       </c>
     </row>
-    <row r="108" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108">
+        <v>456</v>
+      </c>
       <c r="D108">
         <v>456</v>
       </c>
     </row>
-    <row r="109" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109">
+        <v>24</v>
+      </c>
       <c r="D109">
         <v>24</v>
       </c>
     </row>
-    <row r="110" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A110">
+        <v>120</v>
+      </c>
       <c r="D110">
         <v>120</v>
       </c>
     </row>
-    <row r="111" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A111">
+        <v>48</v>
+      </c>
       <c r="D111">
         <v>48</v>
       </c>
     </row>
-    <row r="112" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112">
+        <v>32</v>
+      </c>
       <c r="D112">
         <v>32</v>
       </c>
     </row>
-    <row r="113" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A113">
+        <v>980</v>
+      </c>
       <c r="D113">
         <v>980</v>
       </c>
     </row>
-    <row r="114" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A114">
+        <v>10</v>
+      </c>
       <c r="D114">
         <v>10</v>
       </c>
     </row>
-    <row r="115" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A115">
+        <v>16</v>
+      </c>
       <c r="D115">
         <v>16</v>
       </c>
     </row>
-    <row r="116" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A116">
+        <v>4</v>
+      </c>
       <c r="D116">
         <v>4</v>
       </c>
     </row>
-    <row r="117" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A117">
+        <v>10</v>
+      </c>
       <c r="D117">
         <v>10</v>
       </c>
     </row>
-    <row r="118" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A118">
+        <v>12</v>
+      </c>
       <c r="D118">
         <v>12</v>
       </c>
     </row>
-    <row r="119" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A119">
+        <v>76</v>
+      </c>
       <c r="D119">
         <v>76</v>
       </c>
     </row>
-    <row r="120" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A120">
+        <v>24</v>
+      </c>
       <c r="D120">
         <v>24</v>
       </c>
     </row>
-    <row r="121" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A121">
+        <v>20</v>
+      </c>
       <c r="D121">
         <v>20</v>
       </c>
     </row>
-    <row r="122" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A122">
+        <v>240</v>
+      </c>
       <c r="D122">
         <v>240</v>
       </c>
     </row>
-    <row r="123" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A123">
+        <v>160</v>
+      </c>
       <c r="D123">
         <v>160</v>
       </c>
     </row>
-    <row r="124" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A124">
+        <v>4900</v>
+      </c>
       <c r="D124">
         <v>4900</v>
       </c>
     </row>
-    <row r="125" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A125">
+        <v>50</v>
+      </c>
       <c r="D125">
         <v>50</v>
       </c>
     </row>
-    <row r="126" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A126">
+        <v>80</v>
+      </c>
       <c r="D126">
         <v>80</v>
       </c>
     </row>
-    <row r="127" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A127">
+        <v>20</v>
+      </c>
       <c r="D127">
         <v>20</v>
       </c>
     </row>
-    <row r="128" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A128">
+        <v>50</v>
+      </c>
       <c r="D128">
         <v>50</v>
       </c>
     </row>
-    <row r="129" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A129">
+        <v>60</v>
+      </c>
       <c r="D129">
         <v>60</v>
       </c>
     </row>
-    <row r="130" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A130">
+        <v>380</v>
+      </c>
       <c r="D130">
         <v>380</v>
       </c>
     </row>
-    <row r="131" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A131">
+        <v>120</v>
+      </c>
       <c r="D131">
         <v>120</v>
       </c>
     </row>
-    <row r="132" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A132">
+        <v>20</v>
+      </c>
       <c r="D132">
         <v>20</v>
       </c>

</xml_diff>